<commit_message>
sync main and dev (#11)
* added psutil to install script

* renamed excel folder

* add dependencies

* move to package folder in start file

* add viperbox gui requirement to pyproject

* updated mapping

* added changes to check permanent discharge

* update main to change permanent discharge control

* correct defaults to only set up SU 1

* Remove all mappings to probe number but just keep Channel and OS numbers to fix mapping bug, needs to be reversed, see tag TMPFIX

* trigger bug fixed

* fix empty buffer problem when uploading stimulation settings

---------

Co-authored-by: sbalk <stijn.balk@gmail.com>
</commit_message>
<xml_diff>
--- a/viperboxinterface/defaults/electrode_mapping_short_cables.xlsx
+++ b/viperboxinterface/defaults/electrode_mapping_short_cables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Documents\Projects\NeuraViPeR\NeuraViPeR_once_worked\NeuraViPeR\ViperBoxInterface\defaults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Documents\Projects\NeuraViPeR\NeuraViPeR_once_worked\NeuraViPeR\ViperBoxInterface\viperboxinterface\defaults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A9EFD1-F442-4EE9-8D32-D40FF2AE5BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162D095F-AFAF-4524-A895-14DA385BBB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{BBC9133A-47E8-4183-A3D2-0E13C727BDE7}"/>
   </bookViews>
@@ -3226,7 +3226,7 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
@@ -3749,12 +3749,12 @@
         <v>36</v>
       </c>
       <c r="I10" s="25">
-        <f t="shared" ref="I10:I13" si="6">F10</f>
-        <v>40</v>
+        <f>H10</f>
+        <v>36</v>
       </c>
       <c r="J10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K10" s="23" t="str">
         <f>IF(COUNTIF($I$1:I9,I10)&gt;0, "Duplicate", "Unique")</f>
@@ -3762,11 +3762,11 @@
       </c>
       <c r="L10">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M10" s="25">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N10">
         <f t="shared" si="3"/>
@@ -3803,7 +3803,7 @@
         <v>55</v>
       </c>
       <c r="I11" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="I10:I13" si="6">F11</f>
         <v>62</v>
       </c>
       <c r="J11" s="28">
@@ -4127,28 +4127,28 @@
         <v>51</v>
       </c>
       <c r="I17" s="25">
-        <f t="shared" si="7"/>
-        <v>55</v>
+        <f>H17</f>
+        <v>51</v>
       </c>
       <c r="J17" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K17" s="23" t="str">
         <f>IF(COUNTIF($I$1:I16,I17)&gt;0, "Duplicate", "Unique")</f>
-        <v>Duplicate</v>
-      </c>
-      <c r="L17" t="str">
+        <v>Unique</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M17" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N17" t="str">
+        <v>51</v>
+      </c>
+      <c r="M17" s="25">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="N17">
         <f t="shared" si="3"/>
-        <v/>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
@@ -4514,19 +4514,19 @@
       </c>
       <c r="K24" s="23" t="str">
         <f>IF(COUNTIF($I$1:I23,I24)&gt;0, "Duplicate", "Unique")</f>
-        <v>Duplicate</v>
-      </c>
-      <c r="L24" t="str">
+        <v>Unique</v>
+      </c>
+      <c r="L24">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="M24" s="25" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N24" t="str">
+        <v>40</v>
+      </c>
+      <c r="M24" s="25">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="N24">
         <f t="shared" si="3"/>
-        <v/>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
@@ -4883,12 +4883,12 @@
         <v>57</v>
       </c>
       <c r="I31" s="25">
-        <f t="shared" si="5"/>
-        <v>36</v>
+        <f>H31</f>
+        <v>57</v>
       </c>
       <c r="J31" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K31" s="23" t="str">
         <f>IF(COUNTIF($I$1:I30,I31)&gt;0, "Duplicate", "Unique")</f>
@@ -4896,11 +4896,11 @@
       </c>
       <c r="L31">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="M31" s="25">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N31">
         <f t="shared" si="3"/>
@@ -4991,12 +4991,12 @@
         <v/>
       </c>
       <c r="I33" s="25">
-        <f t="shared" si="5"/>
-        <v>49</v>
+        <f>G33</f>
+        <v>44</v>
       </c>
       <c r="J33" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K33" s="23" t="str">
         <f>IF(COUNTIF($I$1:I32,I33)&gt;0, "Duplicate", "Unique")</f>
@@ -5378,19 +5378,19 @@
       </c>
       <c r="K40" s="23" t="str">
         <f>IF(COUNTIF($I$1:I39,I40)&gt;0, "Duplicate", "Unique")</f>
-        <v>Unique</v>
-      </c>
-      <c r="L40">
+        <v>Duplicate</v>
+      </c>
+      <c r="L40" t="str">
         <f t="shared" si="1"/>
-        <v>51</v>
-      </c>
-      <c r="M40" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N40">
+        <v/>
+      </c>
+      <c r="M40" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N40" t="str">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v/>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
@@ -5864,19 +5864,19 @@
       </c>
       <c r="K49" s="23" t="str">
         <f>IF(COUNTIF($I$1:I48,I49)&gt;0, "Duplicate", "Unique")</f>
-        <v>Unique</v>
-      </c>
-      <c r="L49">
+        <v>Duplicate</v>
+      </c>
+      <c r="L49" t="str">
         <f t="shared" si="1"/>
-        <v>57</v>
-      </c>
-      <c r="M49" s="25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N49">
+        <v/>
+      </c>
+      <c r="M49" s="25" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N49" t="str">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v/>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
@@ -12244,15 +12244,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="f40b0abf-00a2-4b5b-b98d-06c28878d409">
@@ -12268,6 +12259,15 @@
     <TaxCatchAll xmlns="eddb54b3-0260-4a74-8bba-cc772719b91b" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12519,14 +12519,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC23E6A2-90B8-4860-9A82-94B40C6384C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29D9ED97-9FFF-4588-8DC9-F5F025F5C220}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -12534,6 +12526,14 @@
     <ds:schemaRef ds:uri="f40b0abf-00a2-4b5b-b98d-06c28878d409"/>
     <ds:schemaRef ds:uri="82955996-2c56-4dc5-a205-5349b3b0490a"/>
     <ds:schemaRef ds:uri="eddb54b3-0260-4a74-8bba-cc772719b91b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC23E6A2-90B8-4860-9A82-94B40C6384C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>